<commit_message>
adicionado group by - eliminacion de filas repetidas
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Aves</t>
+          <t>Anfibios</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -470,26 +470,26 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Secretario</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -498,26 +498,26 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -526,26 +526,26 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -554,26 +554,26 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pingüino</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -582,26 +582,26 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Guepardo</t>
+          <t>Demonio de Tasmania</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Mofeta</t>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -610,26 +610,26 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Beluga</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Seres humanos</t>
         </is>
       </c>
     </row>
@@ -638,26 +638,26 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -666,26 +666,26 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Tejón</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -694,26 +694,26 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Gavilán pollero</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -722,26 +722,26 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Tiburón toro</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -750,26 +750,26 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Coatí</t>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -778,26 +778,26 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -806,26 +806,26 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -834,26 +834,26 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Visón europeo</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Ratones</t>
         </is>
       </c>
     </row>
@@ -862,26 +862,26 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Perca</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Casuario</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -890,26 +890,26 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Serpiente de coral</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -918,26 +918,26 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -946,26 +946,26 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -974,26 +974,26 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Pavorreales</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>León</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -1002,26 +1002,26 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Nutria</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Mono</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -1030,26 +1030,26 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Tigre siberiano</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Escarabajo de cementerio</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1058,26 +1058,26 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Leopardo</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -1086,22 +1086,26 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Llama</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>Conejo</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Guepardo</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -1110,26 +1114,26 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Orca</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Hámster</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
     </row>
@@ -1138,26 +1142,26 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Orca</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -1166,26 +1170,26 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Serval</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -1194,26 +1198,26 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Lisorofios (extintos)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Milano</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -1222,26 +1226,26 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -1250,26 +1254,26 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Pelícano</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1278,26 +1282,26 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>98</v>
+        <v>32</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -1306,26 +1310,26 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -1334,26 +1338,26 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -1362,26 +1366,26 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -1390,26 +1394,26 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Mapache</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -1418,26 +1422,26 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Labeo bicolor</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -1446,26 +1450,26 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Secretario</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -1474,26 +1478,26 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Tiburón tigre</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -1502,26 +1506,26 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -1530,26 +1534,26 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Secretario</t>
+          <t>Serpiente de coral</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -1558,26 +1562,26 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -1586,26 +1590,26 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Tiburón peregrino</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Cangrejo</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -1614,26 +1618,26 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Gecko leopardo</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -1642,26 +1646,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Antílope</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Perro</t>
-        </is>
-      </c>
+          <t>Canguro</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -1670,26 +1670,26 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Grillo</t>
         </is>
       </c>
     </row>
@@ -1698,26 +1698,26 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Lince</t>
+          <t>Gecko leopardo</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Cucaracha</t>
         </is>
       </c>
     </row>
@@ -1726,26 +1726,26 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Sapos de caña venenosos</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
+          <t>Tigre siberiano</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -1754,26 +1754,26 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>León</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -1782,26 +1782,26 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Murciélago pescador</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -1810,16 +1810,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -1838,26 +1838,26 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Tiburón peregrino</t>
+          <t>Caimán</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -1866,22 +1866,26 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Tapir</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>Caballo</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Cuervo</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Garza real</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1890,11 +1894,11 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1904,12 +1908,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Pez espada</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Pájaro carpintero</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -1918,26 +1922,26 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -1946,26 +1950,26 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Guepardo</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Gallina</t>
+          <t>Cangrejo</t>
         </is>
       </c>
     </row>
@@ -1974,26 +1978,26 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2002,26 +2006,26 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Tigre de bengala</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Grulla</t>
+          <t>Gorila</t>
         </is>
       </c>
     </row>
@@ -2030,26 +2034,26 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Hurón</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -2058,26 +2062,26 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Panda rojo</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -2086,26 +2090,26 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Perro</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2114,26 +2118,26 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Panda rojo</t>
+          <t>Tigre de bengala</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -2142,26 +2146,26 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Lisorofios (extintos)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Linsangs</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -2170,26 +2174,26 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Alimoche</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -2198,11 +2202,11 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2212,12 +2216,12 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Halcón</t>
+          <t>Cobra</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -2226,26 +2230,26 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Linsangs</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Perdiz</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -2254,26 +2258,26 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Tigre siberiano</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -2282,26 +2286,26 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Casuarios</t>
+          <t>Zorrillo</t>
         </is>
       </c>
     </row>
@@ -2310,26 +2314,26 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Gecko leopardo</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -2338,26 +2342,26 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Cóndor andino</t>
+          <t>Búho</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Corydora</t>
+          <t>Cisne</t>
         </is>
       </c>
     </row>
@@ -2366,26 +2370,26 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Mirlo</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -2394,26 +2398,26 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Pez espada</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -2422,26 +2426,26 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Anaconda</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Hormiga</t>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -2450,26 +2454,26 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Perca</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -2478,26 +2482,26 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Hurón</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -2506,26 +2510,26 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Focha</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -2534,26 +2538,26 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Hormiga</t>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -2562,26 +2566,26 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -2594,22 +2598,22 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Lince</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2618,26 +2622,26 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Milano</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Ornitorrinco</t>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -2646,26 +2650,26 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -2674,26 +2678,26 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Lechuza</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -2702,26 +2706,26 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Pez gato</t>
+          <t>Búho</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -2730,26 +2734,26 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Lechuza</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -2758,26 +2762,26 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -2786,26 +2790,26 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Hiena</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -2814,26 +2818,26 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Chacal</t>
+          <t>Beluga</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Morena</t>
         </is>
       </c>
     </row>
@@ -2842,26 +2846,22 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Lisorofios (extintos)</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Ardilla</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Buitre común</t>
-        </is>
-      </c>
+          <t>Koala</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Mofeta</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
     </row>
@@ -2870,26 +2870,26 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Bagre</t>
         </is>
       </c>
     </row>
@@ -2898,11 +2898,11 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2912,12 +2912,12 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Alimoche</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -2926,26 +2926,26 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Lechuza</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -2954,26 +2954,22 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Vaca</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Alimoche</t>
-        </is>
-      </c>
+          <t>Ciervo</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -2982,26 +2978,26 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Morena</t>
+          <t>Corydora</t>
         </is>
       </c>
     </row>
@@ -3010,26 +3006,26 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -3038,26 +3034,26 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Comadreja</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Grillo</t>
         </is>
       </c>
     </row>
@@ -3066,26 +3062,26 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -3094,26 +3090,26 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Pavo real</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -3126,22 +3122,22 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Pavorreales</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Halcón</t>
+          <t>Cóndor andino</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -3150,26 +3146,26 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Corydora</t>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -3178,26 +3174,26 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Muskallonga americano</t>
+          <t>Tollo cigarro</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Mofeta</t>
         </is>
       </c>
     </row>
@@ -3206,26 +3202,26 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Visón europeo</t>
+          <t>Puma</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -3234,26 +3230,22 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Tortuga</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>Gato montés</t>
-        </is>
-      </c>
+          <t>Vaca</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado datasets idbm top 1000 movies y rotten tomates
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Invertebrados</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Herbívoros</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Carnívoros</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Omnívoros</t>
         </is>
@@ -470,26 +475,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Caballito del diablo</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Tollo cigarro</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -498,26 +508,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Piojos</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ballena</t>
+          <t>Cóndor de California</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -526,26 +541,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Ciempiés</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Hámster</t>
+          <t>Salmón</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -554,24 +574,29 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Mariposa limonera</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
+        <is>
+          <t>Albatros</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Cacatúa</t>
         </is>
@@ -582,26 +607,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Cucarachas</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Gallina</t>
+          <t>Pantera negra</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Zorrillo</t>
         </is>
       </c>
     </row>
@@ -610,26 +640,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Avispas excavadoras</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Beluga</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Seres humanos</t>
+          <t>Buitre leonado</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -638,26 +673,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Escarabajo</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Marta</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Serval</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -666,26 +706,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Mariposa del almez</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Fosa</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -694,26 +739,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Curilla o aceitera</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Chacal</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -722,26 +772,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Ciempiés</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Civeta</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -750,26 +805,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Arañas</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Pangolín</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -778,26 +838,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Avispa scolia</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Tigre siberiano</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -806,26 +871,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Cochinillas de humedad</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Cachalote</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -834,26 +904,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Tábano bombilius</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Visón europeo</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Ratones</t>
+          <t>Tiburón toro</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -862,24 +937,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Mariquitas</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Perca</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
+        <is>
+          <t>Ballena azul</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>Langosta</t>
         </is>
@@ -890,26 +970,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Arañas</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>León</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -918,26 +1003,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Avispas portasierra</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Oso pardo</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -946,26 +1036,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Cochinillas</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Piraña</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -974,26 +1069,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Mariquitas</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Cóndor andino</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1002,26 +1102,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Caracoles</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -1030,26 +1135,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Pulgas</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Orca</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -1058,26 +1168,31 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Mariposa dorada</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Milano</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -1086,26 +1201,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Hormigas león</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Guepardo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Gavilán pollero</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -1114,26 +1234,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Curilla o aceitera</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Orca</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Narval</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -1142,26 +1267,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Avispas alfareras</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Orca</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>León</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -1170,26 +1300,31 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Mariposa macaón</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Zorzal</t>
+          <t>Morsa</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -1198,26 +1333,31 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Abejorros</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
+          <t>Ardilla</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Civeta</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Piraña</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -1226,26 +1366,31 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Sapos de caña venenosos</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>Arañas</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>Burro</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Secretario</t>
-        </is>
-      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Grulla</t>
+          <t>Lobo</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -1258,22 +1403,27 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Mariquitas</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Salmón</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Buitre común</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -1282,26 +1432,31 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Mariposa pavo real</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
+          <t>Ciervo</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
           <t>Aguila arpía</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Ratón</t>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -1310,26 +1465,31 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Mariposa saltacercas</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Tiburón blanco</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Cóndor de California</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -1338,7 +1498,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1347,17 +1507,22 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Mariquitas</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Lechuza</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ardilla</t>
         </is>
       </c>
     </row>
@@ -1366,26 +1531,31 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Mariquitas</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Mojarrita</t>
+          <t>Boa</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -1394,26 +1564,31 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Mariposa medioluto</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Delfín</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -1422,26 +1597,31 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Pulgas</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Mojarrita</t>
+          <t>Kinkajú</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -1450,26 +1630,31 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Mariposa sesia</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Gaviota</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -1478,26 +1663,31 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Abejorros</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Civeta</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -1506,26 +1696,31 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Sapos de caña venenosos</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Mariposa ícaro</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Mono</t>
+          <t>Hiena</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -1534,26 +1729,31 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Chinches</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Coyote</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -1562,26 +1762,31 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
+          <t>Ciempiés</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>Llama</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Buitre negro</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Buitre común</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -1590,26 +1795,31 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Abejorros</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Secretario</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -1618,26 +1828,31 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Mariposa macaón</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Boa</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Labeo bicolor</t>
+          <t>Pitón</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -1646,22 +1861,31 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Canguro</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>Grillos</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Tortuga</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Bacalao</t>
+          <t>Buitre leonado</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -1670,26 +1894,31 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Mariposa blanquita de la col</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Cóndor de California</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -1698,26 +1927,31 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Avispas sociales</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Gecko leopardo</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Cucaracha</t>
+          <t>Búho</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -1726,26 +1960,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Mariposa dorada</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Linsangs</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -1754,26 +1993,31 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Libélula emperador</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Tortuga marina</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -1782,26 +2026,31 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Avispas alfareras</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Varano del desierto</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -1810,26 +2059,31 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Mariposa medioluto</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Anaconda</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -1838,26 +2092,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Hormigas</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Hiena</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Morena</t>
         </is>
       </c>
     </row>
@@ -1866,26 +2125,31 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Mariposa lobito agreste</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Serpiente de coral</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -1894,26 +2158,31 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Tábanos</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Erizo</t>
+          <t>Garduña</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -1922,26 +2191,31 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Pulgones</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Nutria</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -1950,26 +2224,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Mariposa cervantes</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Guepardo</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Cangrejo</t>
+          <t>Fosa</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -1978,26 +2257,31 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Chinche roja, zapatero</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Buitre quebrantahuesos</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -2006,26 +2290,31 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Tijeretas</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Gorila</t>
+          <t>Mapache</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -2034,26 +2323,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Avispas excavadoras</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Hurón</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Pangolín</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -2062,26 +2356,31 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Tábano bombilius</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Murciélago espectral</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -2090,26 +2389,31 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Abeja de la miel</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Serpiente de coral</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -2118,26 +2422,31 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Mariposa cervantes</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Visón europeo</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -2146,26 +2455,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Mariposa pavo real</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Langosta</t>
+          <t>Cobra</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2174,26 +2488,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Milpiés</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Alimoche</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Hámster</t>
+          <t>Oso polar</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -2202,26 +2521,31 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Avispas sociales</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Secretario</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Zorrillo</t>
         </is>
       </c>
     </row>
@@ -2230,26 +2554,31 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Abeja de la miel</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Linsangs</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Murciélago pescador</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -2258,26 +2587,31 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Estrellas de mar</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Gavilán pollero</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -2286,26 +2620,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Hormigas león</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Zorrillo</t>
+          <t>Gaviota</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -2314,26 +2653,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Termes</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Lechuza</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -2342,26 +2686,31 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Curilla o aceitera</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Búho</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Cisne</t>
+          <t>Varano del desierto</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -2370,26 +2719,31 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Curilla o aceitera</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Lobo</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -2398,26 +2752,31 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Tábano bombilius</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Pez espada</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Tejón</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -2426,26 +2785,31 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Arañas</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Gavilán pollero</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -2454,26 +2818,31 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Araña de patas largas</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Perca</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Narval</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -2482,26 +2851,31 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Avispas portasierra</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Marta</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Mojarrita</t>
+          <t>Coyote</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -2510,26 +2884,31 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Cigarra o chicharra</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Ballena jorobada</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -2538,26 +2917,31 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Araña cangrejo</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Narval</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Escarabajo de cementerio</t>
         </is>
       </c>
     </row>
@@ -2566,26 +2950,31 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Abejorros</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Marta</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Langosta</t>
+          <t>Alimoche</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -2594,26 +2983,31 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Estrellas de mar</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Fosa</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -2622,26 +3016,31 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Moscardones</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Milano</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Labeo bicolor</t>
+          <t>Muskallonga americano</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -2650,26 +3049,31 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Sapos corredores</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Cochinillas de humedad</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Buitre negro</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -2678,26 +3082,31 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Moscas cernícalo</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Pez espada</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -2706,26 +3115,31 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Grillos</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Búho</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Dragón de Komodo</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -2734,26 +3148,31 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Orugas</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Lechuza</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Ornitorrinco</t>
+          <t>Aguila arpía</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -2762,26 +3181,31 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Escarabajo fitófago</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Leopardo</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Mofeta</t>
         </is>
       </c>
     </row>
@@ -2790,26 +3214,31 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Mariposa ícaro</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Buitre leonado</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -2818,26 +3247,31 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Microsaurios (extintos)</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Avispas portasierra</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Beluga</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Morena</t>
+          <t>Pangolín</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pinzón</t>
         </is>
       </c>
     </row>
@@ -2846,22 +3280,31 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Koala</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr"/>
+          <t>Araña de patas largas</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Oveja</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -2870,26 +3313,31 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Curilla o aceitera</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Bagre</t>
+          <t>Tiburón peregrino</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -2898,26 +3346,31 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
+          <t>Mariposa pavo real</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
           <t>Oveja</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Lobo gris</t>
-        </is>
-      </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Hurón</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2926,26 +3379,31 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Mariposa esfinge colibrí</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Lechuza</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Civeta</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -2954,22 +3412,31 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Ciervo</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr"/>
+          <t>Garrapata</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Vaca</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Zarigüeya</t>
+          <t>Cobra</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -2978,26 +3445,31 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Tábano bombilius</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Corydora</t>
+          <t>Buitre negro</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -3006,26 +3478,31 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Grillos</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -3034,26 +3511,31 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Ajolotes</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Estrellas de mar</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Milano</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -3062,26 +3544,31 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Abeja de la miel</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Caimán</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -3090,26 +3577,31 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Lisorofios (extintos)</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Mariposa ajedrezada menor</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Cacatúa</t>
+          <t>Marlín</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -3118,26 +3610,31 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Chinches</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Cóndor andino</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Bacalao</t>
+          <t>Dragón de Komodo</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Escarabajo de cementerio</t>
         </is>
       </c>
     </row>
@@ -3150,22 +3647,27 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Medusas</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Tiburón martillo</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Petirrojo</t>
+          <t>Coyote</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -3174,26 +3676,31 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Pulgas</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Mofeta</t>
+          <t>Chacal</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -3202,26 +3709,31 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Avispa scolia</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Puma</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Perdiz</t>
+          <t>Cuervo</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -3230,22 +3742,31 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Ranas venenosas</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Vaca</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr"/>
+          <t>Moscas domésticas</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Tapir</t>
+        </is>
+      </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Tortuga lagarto</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionados ejemplos group by
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Anfibios</t>
+          <t>Reptiles</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Invertebrados</t>
+          <t>Rumiantes</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -475,31 +475,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Caballito del diablo</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
+          <t>Buitre quebrantahuesos</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -512,27 +512,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Piojos</t>
+          <t>Apaca</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cóndor de California</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -541,31 +541,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ciempiés</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Salmón</t>
+          <t>Cobra</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -574,31 +574,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Mariposa limonera</t>
+          <t>Urial</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Anaconda</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Cacatúa</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -607,31 +607,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cucarachas</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
+          <t>Barracuda</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Zorrillo</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -640,31 +640,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Avispas excavadoras</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Serval</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Mojarrita</t>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -673,31 +673,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Escarabajo</t>
+          <t>Gacela de Grant</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Garza real</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -706,31 +706,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mariposa del almez</t>
+          <t>Urial</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Hormiga</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -739,31 +739,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Curilla o aceitera</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Chacal</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Gorila</t>
         </is>
       </c>
     </row>
@@ -772,21 +772,21 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ciempiés</t>
+          <t>Nilgó</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -805,31 +805,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Arañas</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -838,31 +838,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Avispa scolia</t>
+          <t>Venado andino</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -871,31 +871,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cochinillas de humedad</t>
+          <t>Venado andino</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Cachalote</t>
+          <t>Linsangs</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -904,31 +904,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Tábano bombilius</t>
+          <t>Nilgó</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -937,31 +937,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Mariquitas</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Langosta</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -970,31 +970,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Arañas</t>
+          <t>Sambar</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -1003,31 +1003,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Avispas portasierra</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -1036,31 +1036,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Cochinillas</t>
+          <t>Bisonte americano</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Serval</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -1069,31 +1069,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mariquitas</t>
+          <t>Sambar</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Cóndor andino</t>
+          <t>Puma</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1102,31 +1102,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Caracoles</t>
+          <t>Bisonte americano</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Visón europeo</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Grulla</t>
+          <t>Ardilla</t>
         </is>
       </c>
     </row>
@@ -1135,31 +1135,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Pulgas</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Orca</t>
+          <t>Comadreja</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1168,31 +1168,31 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Mariposa dorada</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Milano</t>
+          <t>Buitre leonado</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -1201,31 +1201,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Hormigas león</t>
+          <t>Ciervo axis</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -1234,31 +1234,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Curilla o aceitera</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Tortuga carbonaria</t>
         </is>
       </c>
     </row>
@@ -1267,31 +1267,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Avispas alfareras</t>
+          <t>Anoa de montaña</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Murciélago pescador</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Ballena</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -1300,16 +1300,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Mariposa macaón</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1319,12 +1319,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1333,31 +1333,31 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Abejorros</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -1366,31 +1366,31 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Arañas</t>
+          <t>Ciervo de copete</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Labeo bicolor</t>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -1399,31 +1399,31 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Mariquitas</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -1432,31 +1432,31 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Mariposa pavo real</t>
+          <t>Antílope jeroglífico</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -1465,31 +1465,31 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Mariposa saltacercas</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Cóndor de California</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -1498,31 +1498,31 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mariquitas</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Lechuza</t>
+          <t>Tiburón toro</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -1531,31 +1531,31 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Mariquitas</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Boa</t>
+          <t>Buitre leonado</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -1564,31 +1564,31 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Mariposa medioluto</t>
+          <t>Bisonte estepario</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -1597,31 +1597,31 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pulgas</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Kinkajú</t>
+          <t>Gecko leopardo</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -1630,31 +1630,31 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Mariposa sesia</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Caimán</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1663,31 +1663,31 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Abejorros</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Pez gato</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -1696,31 +1696,31 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Mariposa ícaro</t>
+          <t>Alce</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Casuarios</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1729,31 +1729,31 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Chinches</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Varano del desierto</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -1762,31 +1762,31 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Ciempiés</t>
+          <t>Apaca</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Águila pescadora</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Garza real</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -1795,31 +1795,31 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Abejorros</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1828,31 +1828,31 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Mariposa macaón</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Gineta común</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -1861,31 +1861,31 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Grillos</t>
+          <t>Anoa de montaña</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -1894,31 +1894,31 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Tuátaras de Nueva Zelanda</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Mariposa blanquita de la col</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Cóndor de California</t>
+          <t>Anaconda</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -1927,31 +1927,31 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Avispas sociales</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Búho</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Petirrojo</t>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -1960,31 +1960,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Mariposa dorada</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Linsangs</t>
+          <t>Demonio de Tasmania</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -1993,31 +1993,31 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Libélula emperador</t>
+          <t>Bisonte estepario</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Grillo</t>
         </is>
       </c>
     </row>
@@ -2026,31 +2026,31 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Avispas alfareras</t>
+          <t>Gacela de Grant</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Comadreja</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2059,31 +2059,31 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Mariposa medioluto</t>
+          <t>Urial</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Anaconda</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -2092,31 +2092,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Hormigas</t>
+          <t>Antílope de cuatro cuernos</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Morena</t>
+          <t>Gorila</t>
         </is>
       </c>
     </row>
@@ -2125,31 +2125,31 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Mariposa lobito agreste</t>
+          <t>Apaca</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -2158,16 +2158,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Tábanos</t>
+          <t>Alce</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2177,12 +2177,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Tiburón tigre</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -2191,16 +2191,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Pulgones</t>
+          <t>Oryx</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2210,12 +2210,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Pantera negra</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pájaro carpintero</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2224,31 +2224,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Mariposa cervantes</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Pez espada</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -2257,31 +2257,31 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Chinche roja, zapatero</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -2290,31 +2290,31 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Tijeretas</t>
+          <t>Ciervo porcino</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Tortuga lagarto</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -2323,31 +2323,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Avispas excavadoras</t>
+          <t>Ciervo axis</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -2356,16 +2356,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Tábano bombilius</t>
+          <t>Ciervo común</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2375,12 +2375,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Hiena</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -2389,31 +2389,31 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Abeja de la miel</t>
+          <t>Toro</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -2422,31 +2422,31 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Mariposa cervantes</t>
+          <t>Ñu</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Visón europeo</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -2455,31 +2455,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Mariposa pavo real</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Lechuza</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -2488,31 +2488,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Milpiés</t>
+          <t>Ñu</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Casuarios</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -2521,31 +2521,31 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Avispas sociales</t>
+          <t>Gacela de Grant</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Secretario</t>
+          <t>Tiburón toro</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Zorrillo</t>
+          <t>Cuervos</t>
         </is>
       </c>
     </row>
@@ -2554,31 +2554,31 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Abeja de la miel</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Civeta</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -2587,31 +2587,31 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Estrellas de mar</t>
+          <t>Ciervo común</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
+          <t>Fosa</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -2620,31 +2620,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Hormigas león</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -2653,31 +2653,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Termes</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Lechuza</t>
+          <t>Ballena jorobada</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -2686,31 +2686,31 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Curilla o aceitera</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Tejón</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -2719,26 +2719,26 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Curilla o aceitera</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -2752,31 +2752,31 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Tábano bombilius</t>
+          <t>Alce</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Pájaro carpintero</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -2785,31 +2785,31 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Arañas</t>
+          <t>Oryx</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
+          <t>Beluga</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -2818,31 +2818,31 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Araña de patas largas</t>
+          <t>Sitatunga</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Cóndor de California</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Cangrejo</t>
         </is>
       </c>
     </row>
@@ -2851,31 +2851,31 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Avispas portasierra</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Halcón</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -2884,31 +2884,31 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Cigarra o chicharra</t>
+          <t>Nilgó</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Cacatúa</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -2917,31 +2917,31 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Araña cangrejo</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Demonio de Tasmania</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Escarabajo de cementerio</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -2954,27 +2954,27 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Tuátaras de Nueva Zelanda</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Abejorros</t>
+          <t>Gacela de Grant</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Alimoche</t>
+          <t>Perro</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Focha</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -2983,31 +2983,31 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Estrellas de mar</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Murciélago pescador</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -3016,31 +3016,31 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Moscardones</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Muskallonga americano</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -3049,31 +3049,31 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Cochinillas de humedad</t>
+          <t>Bisonte americano</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Varano del desierto</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Petirrojo</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -3082,31 +3082,31 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Moscas cernícalo</t>
+          <t>Alce</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Pez espada</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -3115,31 +3115,31 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Grillos</t>
+          <t>Bongo</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -3148,31 +3148,31 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Orugas</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Orca</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -3181,31 +3181,31 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Escarabajo fitófago</t>
+          <t>Ciervo axis</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Leopardo</t>
+          <t>Mapache</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Mofeta</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -3214,31 +3214,31 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Mariposa ícaro</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Caimán</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Cacatúa</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -3247,31 +3247,31 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Avispas portasierra</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Pingüino</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Pinzón</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -3280,31 +3280,31 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Araña de patas largas</t>
+          <t>Bongo</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -3313,31 +3313,31 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Curilla o aceitera</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Tiburón peregrino</t>
+          <t>Tejón</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Hámster</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -3346,31 +3346,31 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Mariposa pavo real</t>
+          <t>Alce</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Hurón</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -3379,31 +3379,31 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Mariposa esfinge colibrí</t>
+          <t>Antílope de cuatro cuernos</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Varano del desierto</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -3412,31 +3412,31 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Garrapata</t>
+          <t>Venado andino</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Mangosta</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -3445,31 +3445,31 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Tábano bombilius</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -3478,31 +3478,31 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Grillos</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Guepardo</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -3511,31 +3511,31 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Estrellas de mar</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Milano</t>
+          <t>Tigre siberiano</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Ornitorrinco</t>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -3544,31 +3544,31 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Tuátaras de Nueva Zelanda</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Abeja de la miel</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -3577,31 +3577,31 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Mariposa ajedrezada menor</t>
+          <t>Ciervo común</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Perdiz</t>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -3610,31 +3610,31 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Chinches</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Fosa</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Escarabajo de cementerio</t>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -3643,31 +3643,31 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Medusas</t>
+          <t>Sitatunga</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Varano del desierto</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -3676,31 +3676,31 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Pulgas</t>
+          <t>Toro</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Chacal</t>
+          <t>Ballena jorobada</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Mirlo</t>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -3709,31 +3709,31 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Avispa scolia</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -3742,31 +3742,31 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Ranas venenosas</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Moscas domésticas</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
+          <t>Tiburón toro</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado Inplace y metodo query
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Reptiles</t>
+          <t>Vertebrados</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -475,31 +475,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Canguros</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Venado de las Pampas</t>
+          <t>Antílope de cuatro cuernos</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -508,31 +508,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Orcas</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Apaca</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -541,31 +541,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Ñu</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Puma</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Labeo bicolor</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -574,31 +574,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Ñu</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Anaconda</t>
+          <t>León</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Gorila</t>
         </is>
       </c>
     </row>
@@ -607,31 +607,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Anoa de montaña</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Barracuda</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Calamón</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -640,31 +640,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Gorilas</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Bongo</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -673,31 +673,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -706,31 +706,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Tortuga lagarto</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -739,31 +739,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Tiburón blanco</t>
+          <t>Comadreja</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Gorila</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -772,31 +772,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Pingüino</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Langosta</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -805,31 +805,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Bacalaos</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -838,31 +838,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Peces abisales</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Buitre leonado</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -871,31 +871,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Linsangs</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -904,31 +904,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Ranas arcoíris</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Boa</t>
+          <t>Visón europeo</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Tortuga</t>
         </is>
       </c>
     </row>
@@ -937,31 +937,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Venado temazate</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
+          <t>Lechuza</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -970,31 +970,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Capibaras</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sambar</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Mirlo</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -1003,21 +1003,21 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Hienas</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -1036,31 +1036,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Bisonte americano</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Leopardo</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -1069,26 +1069,26 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sambar</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Puma</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1102,31 +1102,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Salamandras gigantes chinas</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bisonte americano</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Visón europeo</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -1135,31 +1135,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Peces espada</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Comadreja</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -1168,31 +1168,31 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Bacalaos</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Kinkajú</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -1201,31 +1201,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Tiburones</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Antílope jeroglífico</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -1234,31 +1234,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Gatos</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Tortuga carbonaria</t>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -1267,31 +1267,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Carpas</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Oryx</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -1300,31 +1300,31 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Gacela de Grant</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Boa</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -1337,27 +1337,27 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Bisonte americano</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Tiburón blanco</t>
+          <t>Nutria</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Coatí</t>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -1366,31 +1366,31 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Tiburones</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Ciervo de copete</t>
+          <t>Sambar</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Serpiente de coral</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -1399,31 +1399,31 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Milano</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -1432,31 +1432,31 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Ballena</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -1465,31 +1465,31 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Pitón</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Petirrojo</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -1498,31 +1498,31 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Peces sapo</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Ratón</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -1531,31 +1531,31 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Mosasaurios (extintos)</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Venado andino</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Panda rojo</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1564,31 +1564,31 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Antílope jeroglífico</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
+          <t>Pantera negra</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -1597,31 +1597,31 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Bongo</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Gecko leopardo</t>
+          <t>Delfín</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -1630,31 +1630,31 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Los tiburones ballena</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Guepardo</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Mofeta</t>
         </is>
       </c>
     </row>
@@ -1663,31 +1663,31 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Pez gato</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Casuarios</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1696,31 +1696,31 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -1729,26 +1729,26 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Venado andino</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Cachalote</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1762,16 +1762,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Apaca</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1781,12 +1781,12 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Águila pescadora</t>
+          <t>Tiburón tigre</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Calamón</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -1795,31 +1795,31 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Orcas</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Leopardo</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -1828,31 +1828,31 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Gineta común</t>
+          <t>Ballena jorobada</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Casuario</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -1861,31 +1861,31 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Salamandras sin pulmón</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Pez espada</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -1894,31 +1894,31 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Anaconda</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -1927,31 +1927,31 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Gorilas</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pájaro carpintero</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -1960,31 +1960,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Pirañas</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Glotón</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Zarigüeya</t>
+          <t>Bagre</t>
         </is>
       </c>
     </row>
@@ -1993,31 +1993,31 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Varano del desierto</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2026,31 +2026,31 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Vacas</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Comadreja</t>
+          <t>Alimoche</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -2059,31 +2059,31 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Orcas</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Bisonte estepario</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Gineta manchada</t>
+          <t>Chacal</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Cangrejo</t>
         </is>
       </c>
     </row>
@@ -2092,31 +2092,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Caballos</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Bisonte americano</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Tiburón blanco</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Gorila</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -2125,21 +2125,21 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Apaca</t>
+          <t>Sambar</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Bacalao</t>
+          <t>Ratones</t>
         </is>
       </c>
     </row>
@@ -2158,31 +2158,31 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Carpas</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Anoa de montaña</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>Lechuza</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -2191,31 +2191,31 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Koi japoneses</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -2224,31 +2224,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Pez espada</t>
+          <t>Leopardo</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -2257,31 +2257,31 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
+          <t>Búfalo cafre</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
           <t>Cabra</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Cebra</t>
-        </is>
-      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Linsangs</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Casuario</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -2290,31 +2290,31 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Carpas</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Ciervo porcino</t>
+          <t>Nilgó</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
+          <t>Mangosta</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -2323,31 +2323,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Delfines</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Ciervo porcino</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Pavo real</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -2356,31 +2356,31 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Petirrojo</t>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -2389,31 +2389,31 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Peces globo</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Caimán</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -2422,31 +2422,31 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Ñu</t>
+          <t>Toro</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2455,31 +2455,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Lechuza</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2488,31 +2488,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Ñu</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -2521,31 +2521,31 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Apaca</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Escarabajo de cementerio</t>
         </is>
       </c>
     </row>
@@ -2554,31 +2554,31 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Leones</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Gayal</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Civeta</t>
+          <t>Pez gato</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -2587,31 +2587,31 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Ranas de Seychelles</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Hormiga</t>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -2620,31 +2620,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Mirlo</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -2653,31 +2653,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -2686,31 +2686,31 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Anoa de montaña</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Coatí</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -2719,31 +2719,31 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Ballenas</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Venado de las Pampas</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Búho</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2752,16 +2752,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Bongo</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2771,12 +2771,12 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -2785,31 +2785,31 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Camaleones</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Beluga</t>
+          <t>Halcón</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -2818,31 +2818,31 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Seres humanos</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Ciervo de copete</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Cóndor de California</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Cangrejo</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -2851,31 +2851,31 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Elefantes</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Halcón</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Pinzón</t>
         </is>
       </c>
     </row>
@@ -2884,31 +2884,31 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Ranas toro africanas</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Coatí</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2917,31 +2917,31 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Bongo</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Faisán</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -2950,31 +2950,31 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Gorilas</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Cuervos</t>
         </is>
       </c>
     </row>
@@ -2983,31 +2983,31 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Ovejas</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Fosa</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -3016,31 +3016,31 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -3049,31 +3049,31 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Bisonte americano</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Perro</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -3082,31 +3082,31 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Mosasaurios (extintos)</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Anoa de montaña</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Visón europeo</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -3115,31 +3115,31 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Bongo</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Boa</t>
+          <t>Nutria</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Perro</t>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -3148,31 +3148,31 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Orca</t>
+          <t>Tortuga lagarto</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -3181,11 +3181,11 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3195,17 +3195,17 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Puma</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -3214,16 +3214,16 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -3233,12 +3233,12 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -3247,31 +3247,31 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Ciervo de copete</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Pingüino</t>
+          <t>Cachalote</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -3280,31 +3280,31 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Bongo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Civeta</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Ballena</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -3313,31 +3313,31 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -3346,31 +3346,31 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Pirañas</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Apaca</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -3379,21 +3379,21 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Camaleones</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Avutarda</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -3412,31 +3412,31 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Tiburones</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Mangosta</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
     </row>
@@ -3445,31 +3445,31 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Apaca</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Narval</t>
+          <t>Buitre quebrantahuesos</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -3478,31 +3478,31 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Necturos</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Guepardo</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -3511,31 +3511,31 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Visón europeo</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -3544,31 +3544,31 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Delfines</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Caimán</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Zarigüeya</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -3577,31 +3577,31 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Celacantos (extintos)</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Tortuga carbonaria</t>
         </is>
       </c>
     </row>
@@ -3610,31 +3610,31 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Elefantes</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Sambar</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -3643,16 +3643,16 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Hienas</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3662,12 +3662,12 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -3676,31 +3676,31 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
+          <t>Tejón</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -3709,31 +3709,31 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -3742,31 +3742,31 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Peces globo</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Barracuda</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ejemplos para joins correctos
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Anfibios</t>
+          <t>Aves</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Rumiantes</t>
+          <t>Herbívoros</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Herbívoros</t>
+          <t>Carnívoros</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Carnívoros</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Omnívoros</t>
         </is>
@@ -475,31 +470,26 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Águila pescadora</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Gaviota</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Cucaracha</t>
+          <t>Ardilla</t>
         </is>
       </c>
     </row>
@@ -508,31 +498,26 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Pantera negra</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tejón</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Morena</t>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -541,31 +526,26 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bongo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>León</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ratón</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -574,31 +554,26 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Ñandú</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -607,31 +582,26 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Lechuzas</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Águila pescadora</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Cangrejo</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -640,31 +610,26 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Glotón</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Erizo</t>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -673,31 +638,26 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Civeta</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Cucaracha</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -706,31 +666,26 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Hiena</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Oso polar</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Avutarda</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -739,31 +694,26 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Apaca</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Marlín</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Avestruz</t>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -772,31 +722,26 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Jaguar</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Pinzón</t>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -805,31 +750,26 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Marabú</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Nutria</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -838,31 +778,26 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Pingüino</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Guepardo</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Hámster</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -871,31 +806,26 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Barracuda</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Avestruz</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -904,31 +834,26 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Pez gato</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Pez arquero</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -937,31 +862,26 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Coyote</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Carpa</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -970,31 +890,26 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Apaca</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Pitón</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Zorro</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -1003,31 +918,26 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Buitre quebrantahuesos</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tiburón peregrino</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Emú</t>
+          <t>Tortuga carbonaria</t>
         </is>
       </c>
     </row>
@@ -1036,31 +946,26 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Marabú</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Pangolín</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Casuario</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -1069,31 +974,26 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Secretario</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Avestruces</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -1102,31 +1002,26 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Tollo cigarro</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Guepardo</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Cacatúa</t>
+          <t>Morena</t>
         </is>
       </c>
     </row>
@@ -1135,31 +1030,26 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Garcilla bueyera</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -1168,31 +1058,26 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Bacalao</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -1201,31 +1086,26 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Pitón</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Gineta común</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Espátula</t>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -1234,31 +1114,26 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Morena</t>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -1267,31 +1142,26 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Ballena jorobada</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Lechuza</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Jabalí</t>
+          <t>Zorrillo</t>
         </is>
       </c>
     </row>
@@ -1304,27 +1174,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Barracuda</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Hámster</t>
+          <t>Morena</t>
         </is>
       </c>
     </row>
@@ -1333,31 +1198,26 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Murciélago pescador</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Anaconda</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Grulla</t>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -1366,31 +1226,26 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Pitón</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Pitón</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Flamingo</t>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -1399,31 +1254,26 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Oso polar</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Grulla</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -1432,31 +1282,26 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Puma</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Manatí</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -1465,31 +1310,26 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Civeta</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Pez arquero</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -1498,31 +1338,26 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Ñu</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Tigre de bengala</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Mapache</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Emú</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -1531,31 +1366,26 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Rinoceronte</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -1564,31 +1394,26 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Sambar</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Tortuga</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -1597,31 +1422,26 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Delfín</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Focha</t>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -1630,31 +1450,26 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>León</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Urraca</t>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -1663,31 +1478,26 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Avispa</t>
+          <t>Ratones</t>
         </is>
       </c>
     </row>
@@ -1696,31 +1506,26 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Gato montés</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Nutria</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -1729,31 +1534,26 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Visón europeo</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Mangosta</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Grulla</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -1762,31 +1562,26 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Narval</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Hormiga</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -1795,31 +1590,26 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Pez globo</t>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -1828,31 +1618,26 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Cobra</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Ornitorrinco</t>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -1861,31 +1646,26 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Nutria</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Chacal</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Tiburón</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -1894,31 +1674,26 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Zorro</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -1927,31 +1702,26 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Ñu</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Pangolín</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Tucán</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -1960,31 +1730,26 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Lechuzas</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Labeo bicolor</t>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -1993,31 +1758,26 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Tiburón peregrino</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Mojarrita</t>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -2026,31 +1786,26 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Cobra</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Tiburón peregrino</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Grajo</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -2059,31 +1814,26 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Perro</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Zarigüeya</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2092,31 +1842,26 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Ñu</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Fosa</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Albatros</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Cuervos</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -2125,31 +1870,26 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Jaguar</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Cucaracha</t>
+          <t>Cisne</t>
         </is>
       </c>
     </row>
@@ -2158,31 +1898,26 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Serpiente de coral</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Ratones</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -2191,31 +1926,26 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Alimoche</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Cuervos</t>
+          <t>Cucaracha</t>
         </is>
       </c>
     </row>
@@ -2224,31 +1954,26 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Ciervo porcino</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Comadreja</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Carpa</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -2257,31 +1982,26 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Venado de las Pampas</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Lechuza</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Focha</t>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -2290,31 +2010,26 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Halcón</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Muskallonga americano</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Ganso</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -2323,31 +2038,26 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Fosa</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Lechuza</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Tiburón</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -2356,31 +2066,26 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Orca</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Pangolín</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Cucaracha</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2389,31 +2094,26 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Marta</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Cerdo</t>
+          <t>Cucaracha</t>
         </is>
       </c>
     </row>
@@ -2422,29 +2122,24 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
-        <is>
-          <t>Beluga</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
         <is>
           <t>Zarigüeya</t>
         </is>
@@ -2455,31 +2150,26 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Foca</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Linsangs</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Pez arquero</t>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -2488,31 +2178,26 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Tiburón tigre</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Delfín</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Perro</t>
+          <t>Bagre</t>
         </is>
       </c>
     </row>
@@ -2521,31 +2206,26 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Alimoche</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Gaviota</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Avestruz</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -2554,31 +2234,26 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Tigre de bengala</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Pez arquero</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -2587,31 +2262,26 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Bacalao</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -2620,31 +2290,26 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Gaviota</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Tortuga carbonaria</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -2653,31 +2318,26 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Sapos corredores</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>León</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Guepardo</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Zorro</t>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -2686,31 +2346,26 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Beluga</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Lince</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Langosta</t>
+          <t>Pez arquero</t>
         </is>
       </c>
     </row>
@@ -2719,31 +2374,26 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Zorzal</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -2752,31 +2402,26 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Perca</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Tejón</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Zorrillo</t>
+          <t>Tortuga</t>
         </is>
       </c>
     </row>
@@ -2785,31 +2430,26 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Piraña</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Flamingo</t>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -2818,31 +2458,26 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Beluga</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Ganso</t>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -2851,31 +2486,26 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Pinzón</t>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -2884,31 +2514,26 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Tigre de bengala</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Buitre común</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>Bacalao</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -2917,31 +2542,26 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Flamingo</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -2950,31 +2570,26 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Lince</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Puma</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Ayeaye</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -2983,31 +2598,26 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Cachalote</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Lechuza</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Pinzón</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -3016,31 +2626,26 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Hurón</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Armadillo</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -3049,31 +2654,26 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Lechuzas</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Barracuda</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Buitre común</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Faisán</t>
+          <t>Pez arquero</t>
         </is>
       </c>
     </row>
@@ -3082,31 +2682,26 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Mangosta</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Escarabajo de cementerio</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -3115,31 +2710,26 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Hurón</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Guepardo</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Cuervos</t>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -3148,31 +2738,26 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Delfín</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Ganso</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -3181,31 +2766,26 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Tollo cigarro</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Lince</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Carpa</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -3214,31 +2794,26 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Cóndor de California</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Hurón</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Ganso</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -3247,31 +2822,26 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Beluga</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Pez gato</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Ardilla</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -3280,31 +2850,26 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Pitón</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Narval</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Gorrión</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -3313,31 +2878,26 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Ranas arcoíris</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Marta</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Bacalao</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -3346,31 +2906,26 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Mapache</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Zarigüeya</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -3379,31 +2934,26 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Gaviota</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Bagre</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -3412,31 +2962,26 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Necturos</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Tortuga lagarto</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Alimoche</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Ganso</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -3445,31 +2990,26 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Microsaurios (extintos)</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Bagre</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -3478,31 +3018,26 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Ajolotes</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Gineta común</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Pez espiga</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -3511,31 +3046,26 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>León</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Búho</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>Hormiga</t>
+          <t>Cangrejo</t>
         </is>
       </c>
     </row>
@@ -3544,31 +3074,26 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Salamandras gigantes chinas</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Demonio de Tasmania</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Pez arquero</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -3577,31 +3102,26 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Milano</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Milano</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Tortuga</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -3610,31 +3130,26 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Marabú</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Gineta manchada</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>Gaviota</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -3643,31 +3158,26 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Salamandras sin pulmón</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Sambar</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Ballena jorobada</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>León marino</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>Coyote</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -3676,31 +3186,26 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Halcón</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Marabú</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>Delfín</t>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -3709,31 +3214,26 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Ranas de Seychelles</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Mangosta</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>Cerdo</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -3742,31 +3242,26 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Ranas toro africanas</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>Humano</t>
+          <t>Piraña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ejemplos para update usando where, inicio funcionapply
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Aves</t>
+          <t>Vertebrados</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rumiantes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Herbívoros</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Carnívoros</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Omnívoros</t>
         </is>
@@ -470,26 +475,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Celacantos (extintos)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Águila pescadora</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>León marino</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -498,26 +508,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Peces espada</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Antílope jeroglífico</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Albatros</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -526,26 +541,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Koi japoneses</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mojarrita</t>
+          <t>Murciélago espectral</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -554,26 +574,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Rinocerontes</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Marta</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Panda rojo</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -582,26 +607,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Urial</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Gineta común</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -610,26 +640,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Tiburones</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Glotón</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Dragón de Komodo</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -638,26 +673,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>Foca</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -666,26 +706,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Atunes</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Erizo</t>
+          <t>Gavilán pollero</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Pinzón</t>
         </is>
       </c>
     </row>
@@ -698,22 +743,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Gato montés</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -722,26 +772,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Sapos de caña venenosos</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Ciervo común</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Gineta manchada</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -750,26 +805,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Marta</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Ballena</t>
+          <t>Mapache</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -778,26 +838,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Esturiones</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Pingüino</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Tortuga marina</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -806,26 +871,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Salmón</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Murciélago espectral</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -834,26 +904,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>Corzuela</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Conejo</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Pez gato</t>
-        </is>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Perca</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -862,26 +937,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Sitatunga</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Tiburón martillo</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Calamón</t>
+          <t>Oso polar</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -890,26 +970,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Lisorofios (extintos)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>Ciervo de copete</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Tortuga</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Pitón</t>
-        </is>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Cacatúa</t>
+          <t>Gineta común</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Pinzón</t>
         </is>
       </c>
     </row>
@@ -918,26 +1003,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Oryx</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tortuga carbonaria</t>
+          <t>Glotón</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -946,26 +1036,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Marabú</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Tigre de bengala</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -974,26 +1069,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Jirafas</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Candelillo</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Buitre negro</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -1002,26 +1102,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Bisonte estepario</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Morena</t>
+          <t>Halcón</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -1030,26 +1135,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Bisonte estepario</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Calamón</t>
+          <t>Tiburón martillo</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -1058,26 +1168,31 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Hámster</t>
+          <t>Orca</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -1086,26 +1201,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Pavorreales</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Ciervo porcino</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Casuarios</t>
+          <t>Comadreja</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -1114,26 +1234,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Pavorreales</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Gallina</t>
+          <t>Caimán</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -1142,26 +1267,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Ciervo axis</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Zorrillo</t>
+          <t>Foca</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -1170,26 +1300,31 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Peces globo</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Barracuda</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Morena</t>
+          <t>Buitre común</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -1198,26 +1333,31 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Venado temazate</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Tiburón blanco</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Avispa</t>
         </is>
       </c>
     </row>
@@ -1226,26 +1366,31 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Pirañas</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>Panda rojo</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -1254,26 +1399,31 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Buitre leonado</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -1282,26 +1432,31 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Puma</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Lince</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -1310,26 +1465,31 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Rinocerontes</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>Sitatunga</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>Alpaca</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Buitre común</t>
-        </is>
-      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Serpiente de coral</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -1338,26 +1498,31 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Peces vela</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Gayal</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Serpiente de coral</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -1366,26 +1531,31 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Gatos</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Jaguar</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Tiburón toro</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -1394,26 +1564,31 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Gatos</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Oso pardo</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -1422,26 +1597,31 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Leopardo</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Mofeta</t>
         </is>
       </c>
     </row>
@@ -1450,26 +1630,31 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Barracuda</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ratones</t>
         </is>
       </c>
     </row>
@@ -1478,26 +1663,31 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>Cobayo</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
           <t>Gaviota</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Ratones</t>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -1506,26 +1696,31 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Koi japoneses</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Focha</t>
+          <t>Caimán</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -1534,24 +1729,29 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Ratones</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Visón europeo</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
+        <is>
+          <t>Buitre común</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>Bengalí rojo</t>
         </is>
@@ -1562,26 +1762,31 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
+          <t>Llama</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>Antílope</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Gineta manchada</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Chacal</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Gatos</t>
         </is>
       </c>
     </row>
@@ -1590,26 +1795,31 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Jaguar</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Serval</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -1618,26 +1828,31 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Ranas de Darwin</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
+          <t>Rinoceronte</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
           <t>Morsa</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Cerdo</t>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Pez arquero</t>
         </is>
       </c>
     </row>
@@ -1646,26 +1861,31 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Zorzal</t>
+          <t>León marino</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -1674,26 +1894,31 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Ciervo axis</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Visón europeo</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -1702,26 +1927,31 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Jirafas</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Hiena</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -1730,26 +1960,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Peces luna</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Garza real</t>
+          <t>Buitre quebrantahuesos</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Pinzón</t>
         </is>
       </c>
     </row>
@@ -1758,26 +1993,31 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Sapos gigantes</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Anoa de llanura</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Tiburón peregrino</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Grulla</t>
+          <t>Serval</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -1786,26 +2026,31 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Anguilas de mar</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Cobra</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Tortuga marina</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ardilla</t>
         </is>
       </c>
     </row>
@@ -1818,22 +2063,27 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Linsangs</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -1842,26 +2092,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Bacalao</t>
+          <t>Albatros</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -1870,26 +2125,31 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Toro</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Cisne</t>
+          <t>Marlín</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -1898,26 +2158,31 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Ciervo de los pantanos</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Varano del desierto</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -1926,26 +2191,31 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Atunes</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Íbice de los Alpes</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Cucaracha</t>
+          <t>Mapache</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -1954,26 +2224,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Sapos de caña venenosos</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Venado temazate</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Boa</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Pavo real</t>
+          <t>Tigre siberiano</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -1986,20 +2261,25 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Antílope de cuatro cuernos</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
+        <is>
+          <t>Buitre negro</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
         <is>
           <t>Oso</t>
         </is>
@@ -2010,26 +2290,31 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Salamandras comunes</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Halcón</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Emú</t>
+          <t>Tiburón toro</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -2038,26 +2323,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Gallipatos</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Fosa</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Tejón</t>
+          <t>Gavilán pollero</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -2066,26 +2356,31 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Orca</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Pitón</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -2094,26 +2389,31 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Marta</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Cucaracha</t>
+          <t>Jaguar</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -2122,26 +2422,27 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Oryx</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Zarigüeya</t>
+          <t>Ciervo</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -2150,26 +2451,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Caimán</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -2178,26 +2484,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Bagre</t>
+          <t>Tigre siberiano</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Grillo</t>
         </is>
       </c>
     </row>
@@ -2206,26 +2517,31 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Orcas</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
+          <t>Alce irlandés</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
           <t>Koala</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Alimoche</t>
-        </is>
-      </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Faisán</t>
+          <t>Gecko leopardo</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -2234,26 +2550,31 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Colibríes</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Pez globo</t>
+          <t>Buitre común</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Carpa</t>
         </is>
       </c>
     </row>
@@ -2262,26 +2583,31 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Tucanes</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Búfalo cafre</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Nutria</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -2290,26 +2616,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Carpas</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Bacalao</t>
+          <t>Cóndor de California</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -2318,26 +2649,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Jirafas</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Venado temazate</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Lobo gris</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Delfín</t>
         </is>
       </c>
     </row>
@@ -2346,26 +2682,31 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Beluga</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Pez arquero</t>
+          <t>Hiena</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -2374,26 +2715,31 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Peces espada</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Langosta</t>
+          <t>Salmón</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -2402,26 +2748,31 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Sapos comunes</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Perca</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Demonio de Tasmania</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -2430,26 +2781,31 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Venado de las Pampas</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Lobo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Tiburón tigre</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -2458,26 +2814,31 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Chimpancés</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Uapití</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Beluga</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Buitre común</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -2486,26 +2847,31 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Cabras</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Gayal</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Tiburón martillo</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2514,26 +2880,31 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Gatos</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Bisonte estepario</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Oso polar</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -2542,26 +2913,31 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Bacalaos</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Gato montés</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Cucaracha</t>
         </is>
       </c>
     </row>
@@ -2570,26 +2946,31 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Capibaras</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Lince</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Gato montés</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -2598,26 +2979,31 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Cachalote</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Tigre siberiano</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -2626,26 +3012,31 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Búfalo de agua</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Coatí</t>
+          <t>Serpiente de coral</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -2654,26 +3045,31 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Bisonte europeo</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Barracuda</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Pez arquero</t>
+          <t>Morsa</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Bagre</t>
         </is>
       </c>
     </row>
@@ -2682,26 +3078,31 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
+          <t>Anoa de montaña</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
           <t>Alpaca</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Tiburón martillo</t>
-        </is>
-      </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Zarigüeya</t>
+          <t>Tigre siberiano</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -2710,26 +3111,31 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Hurón</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Atún</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -2738,26 +3144,31 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Reno</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Hiena</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Grillo</t>
         </is>
       </c>
     </row>
@@ -2766,26 +3177,31 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Lechuzas</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Gamo común</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Tollo cigarro</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Bacalao</t>
+          <t>Tiburón tigre</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -2794,26 +3210,31 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Cóndor de California</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Cachalote</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -2822,26 +3243,31 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Vacas</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Ciervo común</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Beluga</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Ballena azul</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Chimpancé</t>
         </is>
       </c>
     </row>
@@ -2854,22 +3280,27 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Alce irlandés</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Focha</t>
+          <t>Pez espada</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Ardilla</t>
         </is>
       </c>
     </row>
@@ -2878,26 +3309,31 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Buitres</t>
+          <t>Proteos</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Gacela de Grant</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Garduña</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Cocodrilo</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Rinoceronte</t>
         </is>
       </c>
     </row>
@@ -2906,26 +3342,31 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Sitatunga</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Atún</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Zorrillo</t>
         </is>
       </c>
     </row>
@@ -2934,26 +3375,31 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Pelícanos</t>
+          <t>Cecilias</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Pangolín</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Faisán</t>
+          <t>Hiena</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -2962,26 +3408,31 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Vacas</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Impala</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Hámster</t>
+          <t>Cóndor andino</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -2990,26 +3441,31 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Corzo</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Secretario</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Langosta</t>
+          <t>Morsa</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -3018,26 +3474,31 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Las agujas de río</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Ciervo axis</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Ornitorrinco</t>
+          <t>Cuervo</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -3046,26 +3507,31 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Peces globo</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Niala</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Cangrejo</t>
+          <t>Pelícano</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -3074,26 +3540,31 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Sambar</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Jaguar</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Cucaracha</t>
         </is>
       </c>
     </row>
@@ -3102,26 +3573,31 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Vicuña</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Milano</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Casuario</t>
+          <t>Pingüino</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -3130,26 +3606,31 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Peces vela</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Venado andino</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Marabú</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Zarigüeya</t>
+          <t>León</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -3158,26 +3639,31 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Peces vela</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
+          <t>Ciervo de los pantanos</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
           <t>Vaca</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Ballena jorobada</t>
-        </is>
-      </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Tortuga lagarto</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -3186,26 +3672,31 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Ranas arborícolas</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Halcón</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Delfín</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -3214,26 +3705,31 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Avestruces</t>
+          <t>Peces vela</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
+          <t>Corzo</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
           <t>Vaca</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>Lobo gris</t>
-        </is>
-      </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Cóndor andino</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -3242,26 +3738,31 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Koi japoneses</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Cebú</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Gineta manchada</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Pitón</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ejemplos para apply adicionados
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Vertebrados</t>
+          <t>Aves</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Rumiantes</t>
+          <t>Frugívoros</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -475,31 +475,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Celacantos (extintos)</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Murciélago frugívoro</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>León marino</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Flamingo</t>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -508,31 +508,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Peces espada</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Loro</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Cisne</t>
         </is>
       </c>
     </row>
@@ -541,31 +541,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Koi japoneses</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Iguana</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Linsangs</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mirlo</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -574,31 +574,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rinocerontes</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Panda rojo</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Erizo</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -607,31 +607,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pavos</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Lirón</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Gineta común</t>
+          <t>Tiburón toro</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Ratones</t>
         </is>
       </c>
     </row>
@@ -640,31 +640,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tiburones</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Tucán</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
+          <t>Oso pardo</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -673,31 +673,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Murciélago frugívoro</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Halcón</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Hormiga</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -710,27 +710,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Atunes</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pinzón</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -739,31 +739,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Macaco</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Tiburón toro</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Casuarios</t>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -772,31 +772,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Gineta manchada</t>
+          <t>Cobra</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -805,31 +805,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Ganso</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -838,31 +838,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Esturiones</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Chinche del campo</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Gineta común</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -871,31 +871,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -904,31 +904,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Lirón</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Perca</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Gallina</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -937,31 +937,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Tucán</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Oso polar</t>
+          <t>Alimoche</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -970,31 +970,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Lisorofios (extintos)</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Ciervo de copete</t>
+          <t>Perico</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Gineta común</t>
+          <t>Pelícano</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pinzón</t>
+          <t>Corydora</t>
         </is>
       </c>
     </row>
@@ -1003,31 +1003,27 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Pavorreales</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Lémur</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Burro</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Glotón</t>
-        </is>
-      </c>
+          <t>Conejo</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -1036,31 +1032,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Tigre de bengala</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Garcilla bueyera</t>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -1069,31 +1065,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Jirafas</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Buitre leonado</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -1102,16 +1098,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Orangután</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1121,12 +1117,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Halcón</t>
+          <t>Serval</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -1135,31 +1131,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Mono aullador</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Tiburón martillo</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -1168,31 +1164,31 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Mono Tití</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Orca</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -1201,31 +1197,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Ciervo porcino</t>
+          <t>Mosca de la fruta</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Comadreja</t>
+          <t>Marabú</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>Bagre</t>
         </is>
       </c>
     </row>
@@ -1234,16 +1230,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Murciélago frugívoro</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1253,12 +1249,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Jabalí</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -1267,31 +1263,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Gorila</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Foca</t>
+          <t>Gavilán pollero</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Cerdo</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -1300,31 +1296,31 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Peces globo</t>
+          <t>Gallinas</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Tiburón peregrino</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -1333,31 +1329,31 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Macaco</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Tiburón blanco</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Avispa</t>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -1366,16 +1362,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Pirañas</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Perico</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1385,12 +1381,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Panda rojo</t>
+          <t>Alimoche</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -1399,31 +1395,31 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Mono aullador</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
+          <t>Pez gato</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Humano</t>
         </is>
       </c>
     </row>
@@ -1436,27 +1432,27 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Gibón</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Lince</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Cacatúa</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -1465,31 +1461,31 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Rinocerontes</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Bonobo</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Manatí</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -1498,31 +1494,31 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Peces vela</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Gayal</t>
+          <t>Macaco</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Muskallonga americano</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -1531,31 +1527,31 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Tucán</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Tiburón toro</t>
+          <t>Civeta</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Mono</t>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -1564,31 +1560,31 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Perdiz</t>
+          <t>Perezoso</t>
         </is>
       </c>
     </row>
@@ -1597,31 +1593,31 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Águilas</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Lirón</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Leopardo</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Mofeta</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -1630,31 +1626,31 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Tortuga terrestre</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Barracuda</t>
+          <t>Pelícano</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Ratones</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -1663,31 +1659,31 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Anguilas de mar</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Loro</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -1696,31 +1692,31 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Koi japoneses</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Iguana</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Garza real</t>
+          <t>Lémur</t>
         </is>
       </c>
     </row>
@@ -1729,31 +1725,31 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ratones</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Murciélago frugívoro</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Cuervos</t>
         </is>
       </c>
     </row>
@@ -1762,31 +1758,31 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cuervos</t>
+          <t>Lechuzas</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Mosca de la fruta</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Chacal</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -1795,31 +1791,31 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Loros</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Gorila</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Gato montés</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pavo real</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -1828,31 +1824,31 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ranas de Darwin</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Pez arquero</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -1861,21 +1857,21 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Gorila</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1885,7 +1881,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Gorrión</t>
+          <t>Emú</t>
         </is>
       </c>
     </row>
@@ -1894,31 +1890,31 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Cigüeñas</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Loro</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Visón europeo</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pájaro carpintero</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -1927,16 +1923,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Jirafas</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Iguana</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1946,12 +1942,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Pelícano</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -1960,31 +1956,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Peces luna</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Gibón</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Buitre quebrantahuesos</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Pinzón</t>
+          <t>Cuervos</t>
         </is>
       </c>
     </row>
@@ -1993,31 +1989,31 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sapos gigantes</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Macaco</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Serval</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Perdiz</t>
+          <t>Cerdo</t>
         </is>
       </c>
     </row>
@@ -2026,31 +2022,31 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Anguilas de mar</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
+          <t>Tejón</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -2059,31 +2055,31 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Zorro volador</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Linsangs</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -2092,31 +2088,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Orangután</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -2125,31 +2121,31 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Lirón</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Marlín</t>
+          <t>Alimoche</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Ñandú</t>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -2158,16 +2154,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Gorila</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2177,12 +2173,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Varano del desierto</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Gaviota</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -2191,31 +2187,31 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Atunes</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Mapache</t>
+          <t>Pitón</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -2224,31 +2220,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Sapos de caña venenosos</t>
+          <t>Patos</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Tortuga terrestre</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2257,31 +2253,31 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Buitre negro</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Oso</t>
+          <t>Cangrejo</t>
         </is>
       </c>
     </row>
@@ -2290,31 +2286,27 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Salamandras comunes</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Cebra</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Tiburón toro</t>
-        </is>
-      </c>
+          <t>Ciervo</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -2323,31 +2315,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Gallipatos</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Chinche del campo</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Gavilán pollero</t>
+          <t>León</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Hormiga</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -2356,16 +2348,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Mosasaurios (extintos)</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Orangután</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2375,12 +2367,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Murciélago pescador</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Casuario</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -2389,31 +2381,31 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Calandria</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Jaguar</t>
+          <t>Civeta</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Focha</t>
+          <t>Tortuga</t>
         </is>
       </c>
     </row>
@@ -2422,27 +2414,31 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Gaviotas</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Ciervo</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr"/>
+          <t>Tapir</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Mapache</t>
+        </is>
+      </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Lémur</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -2451,31 +2447,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Cóndores</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Iguana</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Caimán</t>
+          <t>Cachalote</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Casuarios</t>
         </is>
       </c>
     </row>
@@ -2484,31 +2480,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Mono aullador</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Jabalí</t>
         </is>
       </c>
     </row>
@@ -2517,31 +2513,31 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Orcas</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Macaco</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Gecko leopardo</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Humano</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -2550,16 +2546,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Pájaros carpinteros</t>
+          <t>Cóndores</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Chinche del campo</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2569,12 +2565,12 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>León marino</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Carpa</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2583,31 +2579,31 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Nutria</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Ayeaye</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -2616,31 +2612,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Carpas</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Cóndor de California</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Mono</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -2649,31 +2645,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Jirafas</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Lémur</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Lobo gris</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Mono</t>
         </is>
       </c>
     </row>
@@ -2682,31 +2678,31 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Pacú</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Gineta común</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -2715,31 +2711,31 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Peces espada</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Conejo del campo</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Salmón</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Tiburón</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -2748,31 +2744,31 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Sapos comunes</t>
+          <t>Pelícanos</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Chimpancé</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
+          <t>Marlín</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -2781,16 +2777,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Venado de las Pampas</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2800,12 +2796,12 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Tortugas</t>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -2814,31 +2810,31 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Chimpancés</t>
+          <t>Guacamayas</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Murciélago frugívoro</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Buitre común</t>
+          <t>Gineta manchada</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Pez espiga</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
     </row>
@@ -2847,31 +2843,31 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Cabras</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Gayal</t>
+          <t>Perico</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Tiburón martillo</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Jerbo</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -2884,17 +2880,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Gatos</t>
+          <t>Águilas</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Mono aullador</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2904,7 +2900,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Grulla</t>
+          <t>Tortugas</t>
         </is>
       </c>
     </row>
@@ -2913,31 +2909,31 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Bacalaos</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Lirón</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Cucaracha</t>
+          <t>Pavo real</t>
         </is>
       </c>
     </row>
@@ -2946,31 +2942,31 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Capibaras</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Gato montés</t>
+          <t>Tollo cigarro</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Espátula</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2979,31 +2975,31 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Gaviotas</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Mono Tití</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Perro</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Urraca</t>
+          <t>Bacalao</t>
         </is>
       </c>
     </row>
@@ -3012,31 +3008,31 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Bonobo</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Zarigüeya</t>
+          <t>Calamón</t>
         </is>
       </c>
     </row>
@@ -3045,31 +3041,31 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Lémur</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Nutria</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Bagre</t>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -3078,31 +3074,31 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Gorila</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
+          <t>Cocodrilo</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Zorro</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -3111,31 +3107,31 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Iguana</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Glotón</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Coyote</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -3144,31 +3140,31 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Gallinas</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Reno</t>
+          <t>Tupaya enana</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Cóndor andino</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Grillo</t>
+          <t>Avestruz</t>
         </is>
       </c>
     </row>
@@ -3177,31 +3173,31 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Lechuzas</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Mono aullador</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Tiburón tigre</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Pájaro carpintero</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -3210,31 +3206,31 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Guacamayas</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Chinche del campo</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Cachalote</t>
+          <t>Cobra</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -3243,31 +3239,31 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Vacas</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Chimpancé</t>
+          <t>Garza real</t>
         </is>
       </c>
     </row>
@@ -3276,26 +3272,26 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Pacú</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Pez espada</t>
+          <t>Comadreja</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3309,31 +3305,31 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Proteos</t>
+          <t>Colibríes</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -3346,27 +3342,27 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Canarios</t>
+          <t>Buitres</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Zorro volador</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Atún</t>
+          <t>Perca</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Zorrillo</t>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -3375,31 +3371,31 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Cecilias</t>
+          <t>Pavos</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Gibón</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Hiena</t>
+          <t>Puma</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Mono</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -3408,31 +3404,31 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Vacas</t>
+          <t>Tucanes</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Mosca de la fruta</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Cóndor andino</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Piraña</t>
+          <t>Ardilla</t>
         </is>
       </c>
     </row>
@@ -3441,31 +3437,31 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Pájaros carpinteros</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Calandria</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Morsa</t>
+          <t>Delfín</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Perezoso</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -3474,31 +3470,31 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Las agujas de río</t>
+          <t>Canarios</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Mono Tití</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Cuervo</t>
+          <t>Lince</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Avestruz</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -3507,31 +3503,31 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Peces globo</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Murciélago frugívoro</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Pelícano</t>
+          <t>Lobo</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Calamón</t>
+          <t>Urraca</t>
         </is>
       </c>
     </row>
@@ -3540,31 +3536,31 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Cigüeñas</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Sambar</t>
+          <t>Tortuga terrestre</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Jaguar</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Cucaracha</t>
+          <t>Pez globo</t>
         </is>
       </c>
     </row>
@@ -3573,31 +3569,31 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Faisanes</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Mono aullador</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Pingüino</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Tucán</t>
+          <t>Coatí</t>
         </is>
       </c>
     </row>
@@ -3606,31 +3602,31 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Peces vela</t>
+          <t>Pavorreales</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Gibón</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>León</t>
+          <t>Pez espada</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -3639,31 +3635,31 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Peces vela</t>
+          <t>Loros</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
+          <t>Aguila arpía</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Grajo</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -3672,31 +3668,31 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Ranas arborícolas</t>
+          <t>Avestruces</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Tapir</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Delfín</t>
+          <t>Pantera negra</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Mosca</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -3705,31 +3701,31 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Peces vela</t>
+          <t>Cuervos</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Mono Tití</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Cóndor andino</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Bengalí rojo</t>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -3738,31 +3734,31 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Koi japoneses</t>
+          <t>Faisanes</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Iguana</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Tortuga</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Pitón</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Armadillo</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionados ejemplos merge eliminacion de columnas repetidas, filtrar con cadena NO sensible al caso
</commit_message>
<xml_diff>
--- a/Pandas/archivos/excel_dataframe.xlsx
+++ b/Pandas/archivos/excel_dataframe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,20 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Rumiantes</t>
+          <t>Herbívoros</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Herbívoros</t>
+          <t>Carnívoros</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Carnívoros</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Omnívoros</t>
         </is>
@@ -475,27 +470,26 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Conejo</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Coyote</t>
+          <t>Delfín</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -504,31 +498,26 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Kinkajú</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Gallina</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -537,31 +526,26 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Perro</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Marlín</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ñandú</t>
+          <t>Pinzón</t>
         </is>
       </c>
     </row>
@@ -570,31 +554,26 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Tortuga lagarto</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Pez gato</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Flamingo</t>
+          <t>Ornitorrinco</t>
         </is>
       </c>
     </row>
@@ -603,31 +582,26 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Tiburón martillo</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Foca</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Coatí</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -636,31 +610,26 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Gineta manchada</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Garza real</t>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -669,31 +638,26 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Coyote</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Ornitorrinco</t>
+          <t>Tortuga carbonaria</t>
         </is>
       </c>
     </row>
@@ -702,31 +666,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Oryx</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Ciervo</t>
-        </is>
-      </c>
+          <t>Elefante</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Jaguar</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Bagre</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -735,31 +690,26 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Focha</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -768,31 +718,26 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Atún</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Kinkajú</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Gorila</t>
+          <t>Avestruces</t>
         </is>
       </c>
     </row>
@@ -801,31 +746,26 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Barracuda</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Gecko leopardo</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Coyote</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -834,31 +774,26 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Gineta común</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Marlín</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Seres humanos</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -867,31 +802,26 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Camaleones</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Mangosta</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Águila pescadora</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Grajo</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -900,31 +830,26 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Lince</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Jerbo</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -933,31 +858,26 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Hurón</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Oso polar</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Coatí</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -966,31 +886,26 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Llama</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Cóndor de California</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Caimán</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Hormiga</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -999,31 +914,26 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Morsa</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Pitón</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Chimpancé</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -1032,31 +942,26 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Leopardo</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Milano</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Garza real</t>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -1065,31 +970,26 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bongo</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Perro</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Ballena</t>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -1098,31 +998,26 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Anaconda</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Murciélago espectral</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Espátula</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1026,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1140,22 +1035,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Corzo</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Marabú</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Águila pescadora</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Casuarios</t>
+          <t>Langosta</t>
         </is>
       </c>
     </row>
@@ -1164,31 +1054,26 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Hiena</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>León marino</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Coatí</t>
+          <t>Avutarda</t>
         </is>
       </c>
     </row>
@@ -1197,31 +1082,26 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Tortugas galápagos</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Kinkajú</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Alimoche</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Morena</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -1230,31 +1110,26 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Cuervo</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Panda rojo</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Avutarda</t>
+          <t>Gaviota</t>
         </is>
       </c>
     </row>
@@ -1263,31 +1138,26 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Venado de las Pampas</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Mangosta</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Milano</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Manatí</t>
+          <t>Nutria</t>
         </is>
       </c>
     </row>
@@ -1296,31 +1166,26 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Armadillo</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -1329,31 +1194,26 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Camaleones</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Barracuda</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Perro</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Hormiga</t>
+          <t>Gallina</t>
         </is>
       </c>
     </row>
@@ -1362,31 +1222,26 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Tigre siberiano</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Cocodrilo</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Garza real</t>
+          <t>Mapache</t>
         </is>
       </c>
     </row>
@@ -1395,31 +1250,26 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Pangolín</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Lince</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Urraca</t>
+          <t>Faisán</t>
         </is>
       </c>
     </row>
@@ -1428,31 +1278,26 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Salmón</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Mangosta</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Cisne</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -1461,31 +1306,26 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Pelícano</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Comadreja</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Bacalao</t>
+          <t>Pez espiga</t>
         </is>
       </c>
     </row>
@@ -1494,31 +1334,26 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Gecko leopardo</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Búho</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Mojarrita</t>
+          <t>Espátula</t>
         </is>
       </c>
     </row>
@@ -1527,31 +1362,26 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Ballena jorobada</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Tortugas</t>
+          <t>Ratón</t>
         </is>
       </c>
     </row>
@@ -1560,31 +1390,26 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Tortuga marina</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Lechuza</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Tortugas</t>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -1593,31 +1418,26 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Aligátores</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Guepardo</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Mangosta</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Zorzal</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -1626,11 +1446,11 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1640,17 +1460,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Pangolín</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Emú</t>
+          <t>Erizo</t>
         </is>
       </c>
     </row>
@@ -1659,31 +1474,26 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Antílope</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Caimán</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Ballena azul</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Ratones</t>
+          <t>Labeo bicolor</t>
         </is>
       </c>
     </row>
@@ -1692,31 +1502,26 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Dinosaurios (extintos)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Ciervo porcino</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Guepardo</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Águila pescadora</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Lémur</t>
+          <t>Cucaracha</t>
         </is>
       </c>
     </row>
@@ -1725,31 +1530,26 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Espátula</t>
+          <t>Ñandú</t>
         </is>
       </c>
     </row>
@@ -1758,31 +1558,26 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Panda rojo</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Murciélago pescador</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Nutria</t>
+          <t>Bagre</t>
         </is>
       </c>
     </row>
@@ -1791,31 +1586,26 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Impala</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Buitre leonado</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Pez globo</t>
+          <t>Pez arquero</t>
         </is>
       </c>
     </row>
@@ -1824,7 +1614,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1833,22 +1623,17 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Mapache</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Pingüino</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Ayeaye</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -1857,31 +1642,26 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Bisonte estepario</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Marabú</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tiburón martillo</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Pavo real</t>
+          <t>Mosca</t>
         </is>
       </c>
     </row>
@@ -1890,31 +1670,26 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Tiburón tigre</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Coyote</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Zarigüeya</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -1923,31 +1698,26 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Pelícano</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Cerdo</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -1956,31 +1726,26 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Jaguar</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Gorrión</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -1989,31 +1754,26 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Ciervo de copete</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Pelícano</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Hormiga</t>
+          <t>Tiburón</t>
         </is>
       </c>
     </row>
@@ -2022,31 +1782,26 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Dragones de Komodo</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Ciervo porcino</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Marlín</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Oso</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -2055,31 +1810,26 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Mangosta</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Oso pardo</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Casuario</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -2088,31 +1838,26 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Alimoche</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Casuarios</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -2121,31 +1866,26 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Bongo</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Tiburón martillo</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Piraña</t>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -2154,31 +1894,26 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Mosasaurios (extintos)</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Buitre quebrantahuesos</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Demonio de Tasmania</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Petirrojo</t>
+          <t>Grajo</t>
         </is>
       </c>
     </row>
@@ -2187,31 +1922,26 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Víboras</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Nutria</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Cuervo</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Mofeta</t>
+          <t>Cacatúa</t>
         </is>
       </c>
     </row>
@@ -2220,31 +1950,26 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Boa</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Delfín</t>
+          <t>Piraña</t>
         </is>
       </c>
     </row>
@@ -2253,31 +1978,26 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Ñu</t>
+          <t>Alpaca</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Águila pescadora</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Fosa</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Chimpancé</t>
+          <t>Ganso</t>
         </is>
       </c>
     </row>
@@ -2286,31 +2006,26 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Orca</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Pingüino</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Pavo real</t>
+          <t>Perro</t>
         </is>
       </c>
     </row>
@@ -2319,31 +2034,26 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Iguanas</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Venado temazate</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Comadreja</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Piraña</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Corydora</t>
+          <t>Ballena</t>
         </is>
       </c>
     </row>
@@ -2352,31 +2062,26 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Bisonte americano</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Tollo cigarro</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Atún</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Tucán</t>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -2385,31 +2090,26 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Camaleones</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Ballena jorobada</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Tortuga</t>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>
@@ -2418,31 +2118,26 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Tuátaras de Nueva Zelanda</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Bisonte americano</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Ardilla</t>
+          <t>Leopardo</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Mapache</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Flamingo</t>
+          <t>Manatí</t>
         </is>
       </c>
     </row>
@@ -2451,31 +2146,26 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Venado andino</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Caballo</t>
+          <t>Piraña</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Beluga</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Gaviota</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -2484,31 +2174,26 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Gineta común</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Linsangs</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Ornitorrinco</t>
+          <t>Grulla</t>
         </is>
       </c>
     </row>
@@ -2517,31 +2202,26 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Búfalo cafre</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Gaviota</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Gato</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Nutria</t>
+          <t>Petirrojo</t>
         </is>
       </c>
     </row>
@@ -2550,31 +2230,26 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Cocodrilos</t>
+          <t>Aligátores</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Koala</t>
+          <t>Murciélago espectral</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Perro</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Tortuga carbonaria</t>
+          <t>Mofeta</t>
         </is>
       </c>
     </row>
@@ -2583,31 +2258,26 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Vaca</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Narval</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Nutria</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Coyote</t>
+          <t>Jerbo</t>
         </is>
       </c>
     </row>
@@ -2616,31 +2286,26 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Tigre de bengala</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Tortuga lagarto</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Pájaro carpintero</t>
+          <t>Tortuga carbonaria</t>
         </is>
       </c>
     </row>
@@ -2649,31 +2314,26 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Serval</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Piraña</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Carpa</t>
+          <t>Flamingo</t>
         </is>
       </c>
     </row>
@@ -2682,31 +2342,26 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Pterosaurios (extintos)</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Ciervo axis</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Oso polar</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Anaconda</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Ratón</t>
+          <t>Oso</t>
         </is>
       </c>
     </row>
@@ -2715,31 +2370,26 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Camaleones</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Llama</t>
+          <t>Cebra</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Águila pescadora</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Tigre siberiano</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Gorrión</t>
+          <t>Mofeta</t>
         </is>
       </c>
     </row>
@@ -2748,31 +2398,26 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Antílope jeroglífico</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Cabra</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Barracuda</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Lémur</t>
+          <t>Pájaro carpintero</t>
         </is>
       </c>
     </row>
@@ -2781,31 +2426,26 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Ciervo común</t>
+          <t>Cabra</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Boa</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Mosca</t>
+          <t>Tucán</t>
         </is>
       </c>
     </row>
@@ -2814,31 +2454,26 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Toro</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Gecko leopardo</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Narval</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Mofeta</t>
+          <t>Escarabajo de cementerio</t>
         </is>
       </c>
     </row>
@@ -2847,31 +2482,26 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Bongo</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Hurón</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Búho</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Avestruz</t>
+          <t>Seres humanos</t>
         </is>
       </c>
     </row>
@@ -2880,31 +2510,26 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Niala</t>
+          <t>Canguro</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Tiburón blanco</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Gineta manchada</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>Zorro</t>
+          <t>Cangrejo</t>
         </is>
       </c>
     </row>
@@ -2913,31 +2538,26 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Mosasaurios (extintos)</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Íbice de los Alpes</t>
+          <t>Tapir</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Glotón</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Serpiente de coral</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Pavo real</t>
+          <t>Armadillo</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2566,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2955,22 +2575,17 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Conejo</t>
+          <t>Boa</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Lince</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Bagre</t>
+          <t>Garcilla bueyera</t>
         </is>
       </c>
     </row>
@@ -2979,31 +2594,26 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Conejo</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Mapache</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Aguila arpía</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Zorzal</t>
+          <t>Cuervos</t>
         </is>
       </c>
     </row>
@@ -3012,31 +2622,26 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Tortugas acuáticas</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Alce irlandés</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Comadreja</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Caimán</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pinzón</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
     </row>
@@ -3045,31 +2650,26 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Mosasaurios (extintos)</t>
+          <t>Basiliscos</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Urial</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Mapache</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Salmón</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Garcilla bueyera</t>
+          <t>Tortuga carbonaria</t>
         </is>
       </c>
     </row>
@@ -3078,31 +2678,26 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Lagartijas comunes</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Gacela de Grant</t>
+          <t>Rinoceronte</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Linsangs</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Pez gato</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Humano</t>
+          <t>Gorrión</t>
         </is>
       </c>
     </row>
@@ -3111,31 +2706,26 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Anoa de montaña</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Cobayo</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Hurón</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Coyote</t>
+          <t>Zorrillo</t>
         </is>
       </c>
     </row>
@@ -3144,31 +2734,26 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Lagartos voladores australianos</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Candelillo</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Perca</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Ratón</t>
+          <t>Casuario</t>
         </is>
       </c>
     </row>
@@ -3177,31 +2762,26 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Koala</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Elefante</t>
+          <t>Milano</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Boa</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pez arquero</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -3210,29 +2790,20 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Dinosaurios (extintos)</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Gayal</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Burro</t>
-        </is>
-      </c>
+          <t>Cobayo</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
-        <is>
-          <t>Mapache</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
         <is>
           <t>Pez arquero</t>
         </is>
@@ -3243,31 +2814,26 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Pterosaurios (extintos)</t>
+          <t>Víboras</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Nilgó</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Secretario</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Pantera negra</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Ratones</t>
+          <t>Mirlo</t>
         </is>
       </c>
     </row>
@@ -3276,31 +2842,26 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Monstruos de Gila</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Gamo común</t>
+          <t>Elefante</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Buitre común</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Kinkajú</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Ornitorrinco</t>
+          <t>Focha</t>
         </is>
       </c>
     </row>
@@ -3309,31 +2870,26 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Alce</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Rinoceronte</t>
+          <t>Pingüino</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Beluga</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Armadillo</t>
+          <t>Morena</t>
         </is>
       </c>
     </row>
@@ -3342,31 +2898,26 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Tuátaras de Nueva Zelanda</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Jirafa</t>
+          <t>Coyote</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Gineta común</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Chimpancé</t>
+          <t>Mojarrita</t>
         </is>
       </c>
     </row>
@@ -3375,31 +2926,26 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Boas constrictoras</t>
+          <t>Monstruos de Gila</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Uapití</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Pingüino</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Pingüino</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Jerbo</t>
+          <t>Perdiz</t>
         </is>
       </c>
     </row>
@@ -3408,31 +2954,26 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Boas constrictoras</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Cebú</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Pez espada</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Buitre común</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Calamón</t>
+          <t>Ayeaye</t>
         </is>
       </c>
     </row>
@@ -3441,31 +2982,26 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Lagartijas comunes</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Búfalo de agua</t>
+          <t>Burro</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Dragón de Komodo</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Civeta</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Coatí</t>
+          <t>Coyote</t>
         </is>
       </c>
     </row>
@@ -3474,31 +3010,26 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Lagartos voladores australianos</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Bisonte europeo</t>
+          <t>Ciervo</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Oso polar</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Zorro</t>
+          <t>Zarigüeya</t>
         </is>
       </c>
     </row>
@@ -3507,31 +3038,26 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Tortugas terrestres</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Oryx</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Burro</t>
+          <t>Demonio de Tasmania</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Tortuga marina</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>Tejón</t>
+          <t>Zorro</t>
         </is>
       </c>
     </row>
@@ -3540,31 +3066,26 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Luciones</t>
+          <t>Varanos</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Antílope de cuatro cuernos</t>
+          <t>Tortuga</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Garduña</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Gato montés</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Calamón</t>
+          <t>Hámster</t>
         </is>
       </c>
     </row>
@@ -3573,31 +3094,26 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Basiliscos</t>
+          <t>Mosasaurios (extintos)</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Oveja</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Canguro</t>
+          <t>Ballena azul</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Perro</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Ñandú</t>
+          <t>Tejón</t>
         </is>
       </c>
     </row>
@@ -3606,31 +3122,26 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Tortugas terrestres</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Sitatunga</t>
+          <t>Cobayo</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Gineta común</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>León</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>Focha</t>
+          <t>Cuervos</t>
         </is>
       </c>
     </row>
@@ -3639,31 +3150,26 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Varanos</t>
+          <t>Luciones</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Vicuña</t>
+          <t>Jirafa</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Antílope</t>
+          <t>Cóndor de California</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Beluga</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>Mosca</t>
+          <t>Zorzal</t>
         </is>
       </c>
     </row>
@@ -3672,31 +3178,26 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Dragones de Komodo</t>
+          <t>Tortugas acuáticas</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Ciervo de copete</t>
+          <t>Vaca</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Oveja</t>
+          <t>Lobo gris</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Serval</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>Mosca</t>
+          <t>Bengalí rojo</t>
         </is>
       </c>
     </row>
@@ -3705,31 +3206,26 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Iguanas</t>
+          <t>Cocodrilos</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Ciervo de los pantanos</t>
+          <t>Caballo</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Ciervo</t>
+          <t>Buitre negro</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Dragón de Komodo</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>Petirrojo</t>
+          <t>Tortuga</t>
         </is>
       </c>
     </row>
@@ -3738,31 +3234,26 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Camaleones</t>
+          <t>Tortugas galápagos</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Anoa de llanura</t>
+          <t>Ardilla</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Cebra</t>
+          <t>Orca</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Lince</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>Jerbo</t>
+          <t>Hormiga</t>
         </is>
       </c>
     </row>

</xml_diff>